<commit_message>
Full working version. Testing still required
</commit_message>
<xml_diff>
--- a/SifterSheetExample.xlsx
+++ b/SifterSheetExample.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\Programming\PythonProjects\EmailSift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9A3E39-5695-43A2-A1BC-FAABA8494DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61E2B3A-81CA-4311-9D4F-F4C879F75786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{740B10AE-0189-40A5-A50B-4518CBC8BA53}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{740B10AE-0189-40A5-A50B-4518CBC8BA53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>samuel.tremblay65@gmail.com</t>
   </si>
@@ -86,6 +88,15 @@
   </si>
   <si>
     <t>Keep from sender</t>
+  </si>
+  <si>
+    <t>emailsift2006@gmail.com</t>
+  </si>
+  <si>
+    <t>peaches</t>
+  </si>
+  <si>
+    <t>banana</t>
   </si>
 </sst>
 </file>
@@ -470,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF8A228-2B2A-4707-9D48-C30D877A3D13}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -542,7 +553,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -583,7 +594,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -625,4 +636,98 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35EF840-7DE2-4F27-A4C4-340AAF934A7D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="intramurals@uottawa.ca" xr:uid="{2071736B-29CD-4FE0-BA5C-981AABC34081}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D27AB7-66E7-414F-915E-43901D2CCA08}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="18.06640625" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" customWidth="1"/>
+    <col min="4" max="4" width="22.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{185CD366-1484-4B47-86F1-6065C0717187}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>